<commit_message>
Fixed issue with single value lists from group level keys
</commit_message>
<xml_diff>
--- a/examples/inventory.xlsx
+++ b/examples/inventory.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joerecchia/Arista/General/ansible-avd-excel-loader/CSVtoAVD/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joerecchia/Arista/General/ansible-avd-excel-loader/CSVtoAVD/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE22961-ADCB-FD42-91C1-BA0A8667683E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6673840C-C030-5D40-83F0-1021C9241766}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="1040" windowWidth="27640" windowHeight="16940" firstSheet="1" activeTab="8" xr2:uid="{71463653-0BCE-624A-9151-A855014D3D36}"/>
+    <workbookView xWindow="2560" yWindow="1040" windowWidth="27640" windowHeight="16940" firstSheet="1" activeTab="3" xr2:uid="{71463653-0BCE-624A-9151-A855014D3D36}"/>
   </bookViews>
   <sheets>
     <sheet name="General Configuration Details" sheetId="5" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="226">
   <si>
     <t>Container Name</t>
   </si>
@@ -378,9 +378,6 @@
     <t>192.168.200.108/24</t>
   </si>
   <si>
-    <t>Ethernet94</t>
-  </si>
-  <si>
     <t>Ethernet4, Ethernet4, Ethernet4, Ethernet4</t>
   </si>
   <si>
@@ -718,6 +715,9 @@
   </si>
   <si>
     <t>Only option is FALSE for now</t>
+  </si>
+  <si>
+    <t>Ethernet3</t>
   </si>
 </sst>
 </file>
@@ -1157,8 +1157,8 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1184,7 +1184,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1208,10 +1208,10 @@
         <v>103</v>
       </c>
       <c r="B5" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="C5" t="s">
         <v>224</v>
-      </c>
-      <c r="C5" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1424,224 +1424,224 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B1" t="s">
         <v>190</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>191</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>192</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>193</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>194</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>186</v>
+      </c>
+      <c r="H1" t="s">
         <v>195</v>
       </c>
-      <c r="G1" t="s">
-        <v>187</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>196</v>
-      </c>
-      <c r="I1" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>203</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>204</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>205</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>206</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>52</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>203</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>204</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="H3" s="6" t="s">
+      <c r="I3" s="6" t="s">
         <v>210</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>203</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>204</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>214</v>
-      </c>
       <c r="G4" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H4" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="I4" s="6" t="s">
         <v>210</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>52</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
       <c r="D6" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>218</v>
-      </c>
       <c r="F6" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H6" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="I6" s="6" t="s">
         <v>210</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>219</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>220</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H7" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="I7" s="6" t="s">
         <v>210</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H8" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="I8" s="6" t="s">
         <v>210</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -1810,9 +1810,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{729B4815-0CB8-AC46-AFED-71170ED8249A}">
   <dimension ref="A1:Z8"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1947,7 +1947,7 @@
         <v>60</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
@@ -1982,7 +1982,7 @@
         <v>60</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
@@ -2002,22 +2002,20 @@
       <c r="E5" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="F5" s="16" t="s">
-        <v>112</v>
-      </c>
+      <c r="F5" s="16"/>
       <c r="G5" s="10">
         <v>65103</v>
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K5" s="11" t="s">
         <v>60</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
@@ -2032,27 +2030,25 @@
         <v>109</v>
       </c>
       <c r="D6" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>112</v>
-      </c>
+      <c r="F6" s="10"/>
       <c r="G6" s="10">
         <v>65103</v>
       </c>
       <c r="H6" s="10"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K6" s="11" t="s">
         <v>60</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
@@ -2095,7 +2091,7 @@
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2146,7 +2142,9 @@
       <c r="A6" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="7"/>
+      <c r="B6" s="7" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="7" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
@@ -2265,31 +2263,31 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>120</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>121</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>62</v>
       </c>
       <c r="I2" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>123</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -2298,28 +2296,28 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>129</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>130</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>62</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -2328,28 +2326,28 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>126</v>
-      </c>
       <c r="D4" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>132</v>
-      </c>
       <c r="F4" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>129</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>130</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>62</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -2363,7 +2361,7 @@
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2452,25 +2450,25 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" t="s">
         <v>135</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>137</v>
       </c>
-      <c r="C1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>138</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G1" t="s">
         <v>139</v>
-      </c>
-      <c r="F1" t="s">
-        <v>145</v>
-      </c>
-      <c r="G1" t="s">
-        <v>140</v>
       </c>
       <c r="H1" t="s">
         <v>63</v>
@@ -2479,18 +2477,18 @@
         <v>20</v>
       </c>
       <c r="J1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B2">
         <v>10000</v>
       </c>
       <c r="C2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D2">
         <v>10</v>
@@ -2499,13 +2497,13 @@
         <v>110</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H2" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="I2" t="s">
         <v>143</v>
-      </c>
-      <c r="I2" t="s">
-        <v>144</v>
       </c>
       <c r="J2" t="b">
         <v>1</v>
@@ -2513,13 +2511,13 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3">
         <v>10000</v>
       </c>
       <c r="C3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D3">
         <v>10</v>
@@ -2531,13 +2529,13 @@
         <v>50111</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J3" t="b">
         <v>1</v>
@@ -2545,13 +2543,13 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B4">
         <v>10000</v>
       </c>
       <c r="C4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D4">
         <v>11</v>
@@ -2561,13 +2559,13 @@
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J4" t="b">
         <v>1</v>
@@ -2575,13 +2573,13 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B5">
         <v>10000</v>
       </c>
       <c r="C5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D5">
         <v>11</v>
@@ -2591,13 +2589,13 @@
       </c>
       <c r="F5" s="19"/>
       <c r="G5" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J5" t="b">
         <v>1</v>
@@ -2605,13 +2603,13 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B6">
         <v>10000</v>
       </c>
       <c r="C6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D6">
         <v>12</v>
@@ -2621,13 +2619,13 @@
       </c>
       <c r="F6" s="19"/>
       <c r="G6" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J6" t="b">
         <v>1</v>
@@ -2635,13 +2633,13 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B7">
         <v>10000</v>
       </c>
       <c r="C7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D7">
         <v>12</v>
@@ -2651,13 +2649,13 @@
       </c>
       <c r="F7" s="19"/>
       <c r="G7" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="H7" s="6" t="s">
-        <v>166</v>
-      </c>
       <c r="I7" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J7" t="b">
         <v>1</v>
@@ -2665,13 +2663,13 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B8">
         <v>10000</v>
       </c>
       <c r="C8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D8">
         <v>13</v>
@@ -2681,13 +2679,13 @@
       </c>
       <c r="F8" s="19"/>
       <c r="G8" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="H8" s="6" t="s">
-        <v>171</v>
-      </c>
       <c r="I8" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J8" t="b">
         <v>1</v>
@@ -2695,13 +2693,13 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B9">
         <v>10000</v>
       </c>
       <c r="C9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D9">
         <v>13</v>
@@ -2711,13 +2709,13 @@
       </c>
       <c r="F9" s="19"/>
       <c r="G9" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="H9" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="H9" s="6" t="s">
-        <v>175</v>
-      </c>
       <c r="I9" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J9" t="b">
         <v>1</v>
@@ -2725,13 +2723,13 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B10">
         <v>10000</v>
       </c>
       <c r="C10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D10">
         <v>14</v>
@@ -2741,13 +2739,13 @@
       </c>
       <c r="F10" s="19"/>
       <c r="G10" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="I10" t="s">
         <v>150</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="I10" t="s">
-        <v>151</v>
       </c>
       <c r="J10" t="b">
         <v>1</v>
@@ -2755,13 +2753,13 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B11">
         <v>20000</v>
       </c>
       <c r="C11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D11">
         <v>20</v>
@@ -2770,13 +2768,13 @@
         <v>210</v>
       </c>
       <c r="G11" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="H11" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="H11" s="6" t="s">
-        <v>153</v>
-      </c>
       <c r="I11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J11" t="b">
         <v>1</v>
@@ -2784,13 +2782,13 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B12">
         <v>20000</v>
       </c>
       <c r="C12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D12">
         <v>20</v>
@@ -2799,13 +2797,13 @@
         <v>211</v>
       </c>
       <c r="G12" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="H12" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="H12" s="6" t="s">
-        <v>155</v>
-      </c>
       <c r="I12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J12" t="b">
         <v>1</v>
@@ -2813,13 +2811,13 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B13">
         <v>20000</v>
       </c>
       <c r="C13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D13">
         <v>21</v>
@@ -2828,13 +2826,13 @@
         <v>250</v>
       </c>
       <c r="G13" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="H13" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="H13" s="6" t="s">
-        <v>157</v>
-      </c>
       <c r="I13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J13" t="b">
         <v>1</v>
@@ -2842,13 +2840,13 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B14">
         <v>30000</v>
       </c>
       <c r="C14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D14">
         <v>30</v>
@@ -2857,13 +2855,13 @@
         <v>310</v>
       </c>
       <c r="G14" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="H14" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="H14" s="6" t="s">
-        <v>159</v>
-      </c>
       <c r="I14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J14" t="b">
         <v>1</v>
@@ -2878,7 +2876,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{397623ED-C334-C646-B5F8-79A547B3D517}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
@@ -2890,32 +2888,32 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B1" t="s">
         <v>187</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>188</v>
-      </c>
-      <c r="C1" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C3" s="6">
         <v>110</v>
@@ -2923,13 +2921,13 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added support for VTEP diagnostics for TENANT_NETWORKS.yml
</commit_message>
<xml_diff>
--- a/examples/inventory.xlsx
+++ b/examples/inventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joerecchia/Arista/General/ansible-avd-excel-loader/CSVtoAVD/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6673840C-C030-5D40-83F0-1021C9241766}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB62C133-017A-CC4C-B933-BB7C43BCEA86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="1040" windowWidth="27640" windowHeight="16940" firstSheet="1" activeTab="3" xr2:uid="{71463653-0BCE-624A-9151-A855014D3D36}"/>
+    <workbookView xWindow="2560" yWindow="1040" windowWidth="27640" windowHeight="16940" xr2:uid="{71463653-0BCE-624A-9151-A855014D3D36}"/>
   </bookViews>
   <sheets>
     <sheet name="General Configuration Details" sheetId="5" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="232">
   <si>
     <t>Container Name</t>
   </si>
@@ -718,13 +718,31 @@
   </si>
   <si>
     <t>Ethernet3</t>
+  </si>
+  <si>
+    <t>VTEP Loopback</t>
+  </si>
+  <si>
+    <t>VTEP Loopback Address Range</t>
+  </si>
+  <si>
+    <t>loopback100</t>
+  </si>
+  <si>
+    <t>10.255.1.0/24</t>
+  </si>
+  <si>
+    <t>hash of cvpadmin password</t>
+  </si>
+  <si>
+    <t>hash of admin password</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -766,35 +784,40 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF005CC5"/>
-      <name val="Consolas"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF0070C0"/>
-      <name val="Consolas"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
+      <color theme="4"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Consolas"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="8"/>
+      <b/>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -817,29 +840,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1156,245 +1180,264 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{293C1073-CE6E-FC49-B936-0C633F8452D0}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15:B17"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="66" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="19" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="15" t="s">
         <v>133</v>
       </c>
+      <c r="C2" s="13"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="15" t="s">
         <v>102</v>
       </c>
+      <c r="C3" s="13"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="15" t="s">
         <v>101</v>
       </c>
+      <c r="C4" s="13"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="13" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="13" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="13" t="s">
         <v>80</v>
       </c>
+      <c r="C7" s="13"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="13" t="s">
         <v>83</v>
       </c>
+      <c r="C8" s="13"/>
     </row>
     <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="20" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="20" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="20" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="10" t="b">
+      <c r="B12" s="15" t="b">
         <v>1</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="20" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="20" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="20" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C15" t="s">
+      <c r="B15" s="15"/>
+      <c r="C15" s="13" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C16" t="s">
+      <c r="B16" s="15"/>
+      <c r="C16" s="13" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C17" t="s">
+      <c r="B17" s="15"/>
+      <c r="C17" s="13" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="A18" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B18" s="15">
         <v>1500</v>
       </c>
+      <c r="C18" s="13"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="A19" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="15">
         <v>1200</v>
       </c>
+      <c r="C19" s="13"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="A20" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B20" s="15">
         <v>1200</v>
       </c>
+      <c r="C20" s="13"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="A21" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="15">
         <v>3</v>
       </c>
+      <c r="C21" s="13"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="A22" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="13" t="s">
         <v>81</v>
       </c>
+      <c r="C22" s="13" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="A23" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="13" t="s">
         <v>82</v>
       </c>
+      <c r="C23" s="13" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="A24" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="13" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="A25" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="C25" t="s">
+      <c r="B25" s="15"/>
+      <c r="C25" s="13" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1409,7 +1452,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1444,203 +1487,205 @@
       <c r="G1" t="s">
         <v>186</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="12" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="14" t="s">
         <v>202</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="14" t="s">
         <v>203</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="13">
         <v>1</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="14" t="s">
         <v>204</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="14" t="s">
         <v>205</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="14" t="s">
         <v>198</v>
       </c>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="14" t="s">
         <v>202</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="14" t="s">
         <v>203</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="13">
         <v>2</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="14" t="s">
         <v>207</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="14" t="s">
         <v>208</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="14" t="s">
         <v>198</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="14" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="14" t="s">
         <v>202</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="14" t="s">
         <v>203</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="13">
         <v>3</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="14" t="s">
         <v>211</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="14" t="s">
         <v>213</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="14" t="s">
         <v>199</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="14" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="14" t="s">
         <v>214</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="14" t="s">
         <v>203</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="13">
         <v>1</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="14" t="s">
         <v>204</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="14" t="s">
         <v>215</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="14" t="s">
         <v>198</v>
       </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="14" t="s">
         <v>214</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="14" t="s">
         <v>203</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="13">
         <v>2</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="14" t="s">
         <v>216</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="14" t="s">
         <v>217</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="14" t="s">
         <v>199</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="14" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="14" t="s">
         <v>218</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="14" t="s">
         <v>219</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="13">
         <v>1</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="14" t="s">
         <v>220</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="14" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="14" t="s">
         <v>221</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="14" t="s">
         <v>219</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="13">
         <v>1</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="14" t="s">
         <v>220</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="14" t="s">
         <v>217</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="14" t="s">
         <v>210</v>
       </c>
     </row>
@@ -1655,7 +1700,7 @@
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1670,13 +1715,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1"/>
@@ -1685,37 +1730,37 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="10">
+    <row r="2" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="15">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="18" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="10">
+    <row r="3" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="15">
         <v>2</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="18" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="10"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="11"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="7"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="10"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="11"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1728,76 +1773,76 @@
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="18" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="18">
         <v>65100</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="18" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="15" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="15" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+    <row r="7" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
+    <row r="8" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="15" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1810,9 +1855,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{729B4815-0CB8-AC46-AFED-71170ED8249A}">
   <dimension ref="A1:Z8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1832,40 +1877,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="9" t="s">
         <v>20</v>
       </c>
       <c r="M1" s="1"/>
@@ -1883,204 +1928,204 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A2" s="10">
+    <row r="2" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="15">
         <v>1</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="15">
         <v>7160</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10">
+      <c r="F2" s="15"/>
+      <c r="G2" s="15">
         <v>65101</v>
       </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6" t="s">
+      <c r="H2" s="15"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="L2" s="18" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A3" s="10">
+    <row r="3" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="15">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="15">
         <v>65102</v>
       </c>
-      <c r="H3" s="10"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6" t="s">
+      <c r="H3" s="15"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="14" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A4" s="10">
+    <row r="4" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="15">
         <f t="shared" ref="A4:A6" si="0">A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="15">
         <v>65102</v>
       </c>
-      <c r="H4" s="10"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6" t="s">
+      <c r="H4" s="15"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="K4" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="L4" s="14" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A5" s="10">
+    <row r="5" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="15">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="F5" s="16"/>
-      <c r="G5" s="10">
+      <c r="F5" s="15"/>
+      <c r="G5" s="15">
         <v>65103</v>
       </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6" t="s">
+      <c r="H5" s="15"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="K5" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="L5" s="6" t="s">
+      <c r="L5" s="14" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A6" s="10">
+    <row r="6" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="15">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10">
+      <c r="F6" s="15"/>
+      <c r="G6" s="15">
         <v>65103</v>
       </c>
-      <c r="H6" s="10"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6" t="s">
+      <c r="H6" s="15"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="K6" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="L6" s="6" t="s">
+      <c r="L6" s="14" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2091,7 +2136,7 @@
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="A2:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2101,96 +2146,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="15" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="15" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="14" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="7"/>
+      <c r="B5" s="16"/>
     </row>
     <row r="6" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="15" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="18" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="15" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="15">
         <v>16384</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="15" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="15" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="B12" s="10" t="b">
+      <c r="B12" s="15" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2205,7 +2250,7 @@
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2245,10 +2290,10 @@
       <c r="G1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="5" t="s">
         <v>75</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -2258,95 +2303,95 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="2" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="13">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="14" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="3" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="13">
         <f>A2+1</f>
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="14" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="4" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="13">
         <f>A3+1</f>
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="14" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2379,44 +2424,44 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="11" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="17"/>
+      <c r="B3" s="11"/>
     </row>
     <row r="4" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="17"/>
+      <c r="B4" s="11"/>
     </row>
     <row r="5" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="7"/>
+      <c r="B5" s="5"/>
     </row>
     <row r="6" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="6">
         <v>16384</v>
       </c>
     </row>
@@ -2427,28 +2472,30 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B85D48BE-CB72-BC43-A02D-945523B5A1A7}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.1640625" customWidth="1"/>
-    <col min="10" max="10" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5" customWidth="1"/>
+    <col min="5" max="5" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>134</v>
       </c>
@@ -2458,412 +2505,453 @@
       <c r="C1" t="s">
         <v>135</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="F1" t="s">
         <v>137</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>138</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>139</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>63</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>20</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="13">
         <v>10000</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="F2" s="13">
         <v>10</v>
       </c>
-      <c r="E2">
+      <c r="G2" s="13">
         <v>110</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="13"/>
+      <c r="I2" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="J2" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="J2" t="b">
+      <c r="L2" s="13" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="13">
         <v>10000</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13">
         <v>10</v>
       </c>
-      <c r="E3">
+      <c r="G3" s="13">
         <v>111</v>
       </c>
-      <c r="F3" s="19">
+      <c r="H3" s="14">
         <v>50111</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="I3" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="J3" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="J3" t="b">
+      <c r="L3" s="13" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="13">
         <v>10000</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13">
         <v>11</v>
       </c>
-      <c r="E4">
+      <c r="G4" s="13">
         <v>120</v>
       </c>
-      <c r="F4" s="19"/>
-      <c r="G4" s="6" t="s">
+      <c r="H4" s="14"/>
+      <c r="I4" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="J4" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="J4" t="b">
+      <c r="L4" s="13" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="13">
         <v>10000</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13">
         <v>11</v>
       </c>
-      <c r="E5">
+      <c r="G5" s="13">
         <v>121</v>
       </c>
-      <c r="F5" s="19"/>
-      <c r="G5" s="6" t="s">
+      <c r="H5" s="14"/>
+      <c r="I5" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="J5" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K5" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="J5" t="b">
+      <c r="L5" s="13" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="13">
         <v>10000</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="13" t="s">
         <v>180</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13">
         <v>12</v>
       </c>
-      <c r="E6">
+      <c r="G6" s="13">
         <v>130</v>
       </c>
-      <c r="F6" s="19"/>
-      <c r="G6" s="6" t="s">
+      <c r="H6" s="14"/>
+      <c r="I6" s="14" t="s">
         <v>163</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="J6" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="K6" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="J6" t="b">
+      <c r="L6" s="13" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="13">
         <v>10000</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="13" t="s">
         <v>180</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13">
         <v>12</v>
       </c>
-      <c r="E7">
+      <c r="G7" s="13">
         <v>131</v>
       </c>
-      <c r="F7" s="19"/>
-      <c r="G7" s="6" t="s">
+      <c r="H7" s="14"/>
+      <c r="I7" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="J7" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="K7" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="J7" t="b">
+      <c r="L7" s="13" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="13">
         <v>10000</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13">
         <v>13</v>
       </c>
-      <c r="E8">
+      <c r="G8" s="13">
         <v>140</v>
       </c>
-      <c r="F8" s="19"/>
-      <c r="G8" s="6" t="s">
+      <c r="H8" s="14"/>
+      <c r="I8" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="J8" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="K8" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="J8" t="b">
+      <c r="L8" s="13" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="13">
         <v>10000</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13">
         <v>13</v>
       </c>
-      <c r="E9">
+      <c r="G9" s="13">
         <v>141</v>
       </c>
-      <c r="F9" s="19"/>
-      <c r="G9" s="6" t="s">
+      <c r="H9" s="14"/>
+      <c r="I9" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="J9" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="K9" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="J9" t="b">
+      <c r="L9" s="13" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="13">
         <v>10000</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13">
         <v>14</v>
       </c>
-      <c r="E10">
+      <c r="G10" s="13">
         <v>150</v>
       </c>
-      <c r="F10" s="19"/>
-      <c r="G10" s="6" t="s">
+      <c r="H10" s="14"/>
+      <c r="I10" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="J10" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="I10" t="s">
+      <c r="K10" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="J10" t="b">
+      <c r="L10" s="13" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="13">
         <v>20000</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13">
         <v>20</v>
       </c>
-      <c r="E11">
+      <c r="G11" s="13">
         <v>210</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="H11" s="13"/>
+      <c r="I11" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="J11" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="I11" t="s">
+      <c r="K11" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="J11" t="b">
+      <c r="L11" s="13" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="13">
         <v>20000</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13">
         <v>20</v>
       </c>
-      <c r="E12">
+      <c r="G12" s="13">
         <v>211</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="H12" s="13"/>
+      <c r="I12" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="J12" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="I12" t="s">
+      <c r="K12" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="J12" t="b">
+      <c r="L12" s="13" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="13">
         <v>20000</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13">
         <v>21</v>
       </c>
-      <c r="E13">
+      <c r="G13" s="13">
         <v>250</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="H13" s="13"/>
+      <c r="I13" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="J13" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="I13" t="s">
+      <c r="K13" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="J13" t="b">
+      <c r="L13" s="13" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="13">
         <v>30000</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13">
         <v>30</v>
       </c>
-      <c r="E14">
+      <c r="G14" s="13">
         <v>310</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="H14" s="13"/>
+      <c r="I14" s="14" t="s">
         <v>157</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="J14" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="I14" t="s">
+      <c r="K14" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="J14" t="b">
+      <c r="L14" s="13" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2878,7 +2966,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2898,35 +2986,35 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="14" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="14" t="s">
         <v>198</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="14">
         <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="14" t="s">
         <v>199</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="14" t="s">
         <v>201</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed loopback interface syntax issue
</commit_message>
<xml_diff>
--- a/examples/inventory.xlsx
+++ b/examples/inventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joerecchia/Arista/General/ansible-avd-excel-loader/CSVtoAVD/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB62C133-017A-CC4C-B933-BB7C43BCEA86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750BDAAF-C5CE-CD41-84E3-5C2210BDB58E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="1040" windowWidth="27640" windowHeight="16940" xr2:uid="{71463653-0BCE-624A-9151-A855014D3D36}"/>
+    <workbookView xWindow="2560" yWindow="1040" windowWidth="27640" windowHeight="16940" activeTab="7" xr2:uid="{71463653-0BCE-624A-9151-A855014D3D36}"/>
   </bookViews>
   <sheets>
     <sheet name="General Configuration Details" sheetId="5" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="231">
   <si>
     <t>Container Name</t>
   </si>
@@ -724,9 +724,6 @@
   </si>
   <si>
     <t>VTEP Loopback Address Range</t>
-  </si>
-  <si>
-    <t>loopback100</t>
   </si>
   <si>
     <t>10.255.1.0/24</t>
@@ -1180,7 +1177,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{293C1073-CE6E-FC49-B936-0C633F8452D0}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
@@ -1407,7 +1404,7 @@
         <v>81</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -1418,7 +1415,7 @@
         <v>82</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -2474,9 +2471,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B85D48BE-CB72-BC43-A02D-945523B5A1A7}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2543,11 +2540,11 @@
       <c r="C2" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="13">
+        <v>100</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>228</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>229</v>
       </c>
       <c r="F2" s="13">
         <v>10</v>

</xml_diff>

<commit_message>
Added option to Tenants tab for 'ip address virtual' as well as 'virtual router address'
</commit_message>
<xml_diff>
--- a/examples/inventory.xlsx
+++ b/examples/inventory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joerecchia/Arista/General/ansible-avd-excel-loader/CSVtoAVD/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750BDAAF-C5CE-CD41-84E3-5C2210BDB58E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE7E8C5-89DD-4D4D-99C3-81C8EEC98C78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="1040" windowWidth="27640" windowHeight="16940" activeTab="7" xr2:uid="{71463653-0BCE-624A-9151-A855014D3D36}"/>
+    <workbookView xWindow="13160" yWindow="1220" windowWidth="20240" windowHeight="15700" firstSheet="2" activeTab="7" xr2:uid="{71463653-0BCE-624A-9151-A855014D3D36}"/>
   </bookViews>
   <sheets>
     <sheet name="General Configuration Details" sheetId="5" r:id="rId1"/>
@@ -29,18 +29,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="234">
   <si>
     <t>Container Name</t>
   </si>
@@ -459,15 +453,9 @@
     <t>SVI</t>
   </si>
   <si>
-    <t>SVI Address</t>
-  </si>
-  <si>
     <t>Enabled</t>
   </si>
   <si>
-    <t>10.1.11.1/24</t>
-  </si>
-  <si>
     <t>Tenant_A_OP_Zone_1</t>
   </si>
   <si>
@@ -477,45 +465,21 @@
     <t>Vlan VNI Override</t>
   </si>
   <si>
-    <t>10.1.10.1/24</t>
-  </si>
-  <si>
-    <t>10.1.20.1/24</t>
-  </si>
-  <si>
     <t>Tenant_A_OP_Zone_2</t>
   </si>
   <si>
-    <t>10.1.21.1/24</t>
-  </si>
-  <si>
-    <t>10.1.50.1/24</t>
-  </si>
-  <si>
     <t>wan</t>
   </si>
   <si>
-    <t>10.2.10.1/24</t>
-  </si>
-  <si>
     <t>Tenant_B_OP_Zone_1</t>
   </si>
   <si>
-    <t>10.2.11.1/24</t>
-  </si>
-  <si>
     <t>Tenant_B_OP_Zone_2</t>
   </si>
   <si>
-    <t>10.2.50.1/24</t>
-  </si>
-  <si>
     <t>Tenant_B_WAN_Zone_1</t>
   </si>
   <si>
-    <t>10.3.10.1/24</t>
-  </si>
-  <si>
     <t>Tenant_C_OP_Zone_1</t>
   </si>
   <si>
@@ -531,12 +495,6 @@
     <t>app, erp1</t>
   </si>
   <si>
-    <t>10.1.30.1/24</t>
-  </si>
-  <si>
-    <t>10.1.31.1/24</t>
-  </si>
-  <si>
     <t>Tenant_A_APP_Zone_2</t>
   </si>
   <si>
@@ -549,9 +507,6 @@
     <t>Tenant_A_DB_Zone</t>
   </si>
   <si>
-    <t>10.1.40.1/24</t>
-  </si>
-  <si>
     <t>Tenant_A_DB_Zone_1</t>
   </si>
   <si>
@@ -561,9 +516,6 @@
     <t>db</t>
   </si>
   <si>
-    <t>10.1.41.1/24</t>
-  </si>
-  <si>
     <t>Tenant_A_DB_Zone_2</t>
   </si>
   <si>
@@ -733,6 +685,57 @@
   </si>
   <si>
     <t>hash of admin password</t>
+  </si>
+  <si>
+    <t>IP Address Virtual</t>
+  </si>
+  <si>
+    <t>Virtual IP Subnet</t>
+  </si>
+  <si>
+    <t>Virtual Router Address</t>
+  </si>
+  <si>
+    <t>Virtual Address Type</t>
+  </si>
+  <si>
+    <t>10.1.11.0/24</t>
+  </si>
+  <si>
+    <t>10.1.10.0/24</t>
+  </si>
+  <si>
+    <t>10.1.20.0/24</t>
+  </si>
+  <si>
+    <t>10.1.21.0/24</t>
+  </si>
+  <si>
+    <t>10.1.30.0/24</t>
+  </si>
+  <si>
+    <t>10.1.31.0/24</t>
+  </si>
+  <si>
+    <t>10.1.40.0/24</t>
+  </si>
+  <si>
+    <t>10.1.41.0/24</t>
+  </si>
+  <si>
+    <t>10.1.50.0/24</t>
+  </si>
+  <si>
+    <t>10.2.10.0/24</t>
+  </si>
+  <si>
+    <t>10.2.11.0/24</t>
+  </si>
+  <si>
+    <t>10.2.50.0/24</t>
+  </si>
+  <si>
+    <t>10.3.10.0/24</t>
   </si>
 </sst>
 </file>
@@ -1232,10 +1235,10 @@
         <v>103</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1404,7 +1407,7 @@
         <v>81</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -1415,7 +1418,7 @@
         <v>82</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -1464,226 +1467,226 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="B1" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="C1" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="D1" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="E1" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="F1" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="G1" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="C2" s="13">
         <v>1</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="F2" s="14" t="s">
         <v>52</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="H2" s="13"/>
       <c r="I2" s="13"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="C3" s="13">
         <v>2</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="C4" s="13">
         <v>3</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="C5" s="13">
         <v>1</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="F5" s="14" t="s">
         <v>52</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="C6" s="13">
         <v>2</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="F6" s="14" t="s">
         <v>120</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="C7" s="13">
         <v>1</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="F7" s="14" t="s">
         <v>129</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="C8" s="13">
         <v>1</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="F8" s="14" t="s">
         <v>129</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -1852,9 +1855,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{729B4815-0CB8-AC46-AFED-71170ED8249A}">
   <dimension ref="A1:Z8"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView topLeftCell="I1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1989,7 +1992,7 @@
         <v>60</v>
       </c>
       <c r="L3" s="14" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -2024,7 +2027,7 @@
         <v>60</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -2057,7 +2060,7 @@
         <v>60</v>
       </c>
       <c r="L5" s="14" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -2090,7 +2093,7 @@
         <v>60</v>
       </c>
       <c r="L6" s="14" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
@@ -2131,7 +2134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E05D6DD-4109-2F48-82B0-171BA5DAA88E}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView topLeftCell="I1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B12" sqref="A2:B12"/>
     </sheetView>
@@ -2185,7 +2188,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2469,11 +2472,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B85D48BE-CB72-BC43-A02D-945523B5A1A7}">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="110" zoomScaleNormal="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2486,13 +2489,14 @@
     <col min="6" max="6" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>134</v>
       </c>
@@ -2503,10 +2507,10 @@
         <v>135</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="F1" t="s">
         <v>137</v>
@@ -2515,22 +2519,25 @@
         <v>138</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="I1" t="s">
+        <v>220</v>
+      </c>
+      <c r="J1" t="s">
+        <v>218</v>
+      </c>
+      <c r="K1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" t="s">
         <v>139</v>
       </c>
-      <c r="J1" t="s">
-        <v>63</v>
-      </c>
-      <c r="K1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>122</v>
       </c>
@@ -2538,13 +2545,13 @@
         <v>10000</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="D2" s="13">
         <v>100</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="F2" s="13">
         <v>10</v>
@@ -2554,19 +2561,22 @@
       </c>
       <c r="H2" s="13"/>
       <c r="I2" s="14" t="s">
-        <v>145</v>
+        <v>217</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="K2" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="L2" s="13" t="b">
+        <v>222</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="M2" s="13" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>122</v>
       </c>
@@ -2574,7 +2584,7 @@
         <v>10000</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="D3" s="13"/>
       <c r="E3" s="13"/>
@@ -2588,19 +2598,22 @@
         <v>50111</v>
       </c>
       <c r="I3" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="L3" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="J3" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="K3" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="L3" s="13" t="b">
+      <c r="M3" s="13" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>122</v>
       </c>
@@ -2608,7 +2621,7 @@
         <v>10000</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="13"/>
@@ -2620,19 +2633,22 @@
       </c>
       <c r="H4" s="14"/>
       <c r="I4" s="14" t="s">
-        <v>146</v>
+        <v>217</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="K4" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="L4" s="13" t="b">
+        <v>223</v>
+      </c>
+      <c r="K4" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="M4" s="13" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>122</v>
       </c>
@@ -2640,7 +2656,7 @@
         <v>10000</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -2652,19 +2668,22 @@
       </c>
       <c r="H5" s="14"/>
       <c r="I5" s="14" t="s">
-        <v>148</v>
+        <v>217</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="K5" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="L5" s="13" t="b">
+        <v>224</v>
+      </c>
+      <c r="K5" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="M5" s="13" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>122</v>
       </c>
@@ -2672,7 +2691,7 @@
         <v>10000</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
@@ -2684,19 +2703,22 @@
       </c>
       <c r="H6" s="14"/>
       <c r="I6" s="14" t="s">
-        <v>163</v>
+        <v>217</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>171</v>
+        <v>225</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="L6" s="13" t="b">
+        <v>158</v>
+      </c>
+      <c r="L6" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="M6" s="13" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>122</v>
       </c>
@@ -2704,7 +2726,7 @@
         <v>10000</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
@@ -2716,19 +2738,22 @@
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="14" t="s">
-        <v>164</v>
+        <v>217</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>165</v>
+        <v>226</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="L7" s="13" t="b">
+        <v>153</v>
+      </c>
+      <c r="L7" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="M7" s="13" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>122</v>
       </c>
@@ -2736,7 +2761,7 @@
         <v>10000</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
@@ -2748,19 +2773,22 @@
       </c>
       <c r="H8" s="14"/>
       <c r="I8" s="14" t="s">
-        <v>169</v>
+        <v>217</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>170</v>
+        <v>227</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="L8" s="13" t="b">
+        <v>157</v>
+      </c>
+      <c r="L8" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="M8" s="13" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>122</v>
       </c>
@@ -2768,7 +2796,7 @@
         <v>10000</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
@@ -2780,19 +2808,22 @@
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>173</v>
+        <v>217</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>174</v>
+        <v>228</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="L9" s="13" t="b">
+        <v>160</v>
+      </c>
+      <c r="L9" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="M9" s="13" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>122</v>
       </c>
@@ -2800,7 +2831,7 @@
         <v>10000</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
@@ -2812,27 +2843,30 @@
       </c>
       <c r="H10" s="14"/>
       <c r="I10" s="14" t="s">
-        <v>149</v>
+        <v>217</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>185</v>
-      </c>
-      <c r="K10" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="L10" s="13" t="b">
+        <v>229</v>
+      </c>
+      <c r="K10" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="L10" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="M10" s="13" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="B11" s="13">
         <v>20000</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
@@ -2844,27 +2878,30 @@
       </c>
       <c r="H11" s="13"/>
       <c r="I11" s="14" t="s">
-        <v>151</v>
+        <v>217</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="K11" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="L11" s="13" t="b">
+        <v>230</v>
+      </c>
+      <c r="K11" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="L11" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="M11" s="13" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="B12" s="13">
         <v>20000</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
@@ -2876,27 +2913,30 @@
       </c>
       <c r="H12" s="13"/>
       <c r="I12" s="14" t="s">
-        <v>153</v>
+        <v>217</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="K12" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="L12" s="13" t="b">
+        <v>231</v>
+      </c>
+      <c r="K12" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="L12" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="M12" s="13" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="B13" s="13">
         <v>20000</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
@@ -2908,27 +2948,30 @@
       </c>
       <c r="H13" s="13"/>
       <c r="I13" s="14" t="s">
-        <v>155</v>
+        <v>217</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="K13" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="L13" s="13" t="b">
+        <v>232</v>
+      </c>
+      <c r="K13" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="L13" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="M13" s="13" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="B14" s="13">
         <v>30000</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
@@ -2940,15 +2983,18 @@
       </c>
       <c r="H14" s="13"/>
       <c r="I14" s="14" t="s">
-        <v>157</v>
+        <v>217</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="K14" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="L14" s="13" t="b">
+        <v>233</v>
+      </c>
+      <c r="K14" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="L14" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="M14" s="13" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2973,32 +3019,32 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="B1" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="C1" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="C3" s="14">
         <v>110</v>
@@ -3006,13 +3052,13 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed issue for no leafs provided in spreadsheet
</commit_message>
<xml_diff>
--- a/examples/inventory.xlsx
+++ b/examples/inventory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joerecchia/Arista/General/ansible-avd-excel-loader/CSVtoAVD/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE7E8C5-89DD-4D4D-99C3-81C8EEC98C78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7BB021A-848A-204A-A23A-600341041057}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13160" yWindow="1220" windowWidth="20240" windowHeight="15700" firstSheet="2" activeTab="7" xr2:uid="{71463653-0BCE-624A-9151-A855014D3D36}"/>
+    <workbookView xWindow="820" yWindow="900" windowWidth="32200" windowHeight="17020" xr2:uid="{71463653-0BCE-624A-9151-A855014D3D36}"/>
   </bookViews>
   <sheets>
     <sheet name="General Configuration Details" sheetId="5" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="238">
   <si>
     <t>Container Name</t>
   </si>
@@ -339,12 +339,6 @@
     <t>BGP wait-for-convergence</t>
   </si>
   <si>
-    <t>DC2</t>
-  </si>
-  <si>
-    <t>DC2_AVD</t>
-  </si>
-  <si>
     <t>Validate Network with Batfish</t>
   </si>
   <si>
@@ -435,9 +429,6 @@
     <t>Ethernet8, Ethernet8</t>
   </si>
   <si>
-    <t>DC2-Fabric</t>
-  </si>
-  <si>
     <t>Tenant</t>
   </si>
   <si>
@@ -693,9 +684,6 @@
     <t>Virtual IP Subnet</t>
   </si>
   <si>
-    <t>Virtual Router Address</t>
-  </si>
-  <si>
     <t>Virtual Address Type</t>
   </si>
   <si>
@@ -736,6 +724,30 @@
   </si>
   <si>
     <t>10.3.10.0/24</t>
+  </si>
+  <si>
+    <t>IP Virtual Router Address</t>
+  </si>
+  <si>
+    <t>avd</t>
+  </si>
+  <si>
+    <t>#Root container</t>
+  </si>
+  <si>
+    <t>#Device filter</t>
+  </si>
+  <si>
+    <t>AVD-Demo</t>
+  </si>
+  <si>
+    <t>#prefx for configlet i.e. If device name is 'lf1' the configlet name will be 'avd_lf1'</t>
+  </si>
+  <si>
+    <t>DNS Servers separated by a comma</t>
+  </si>
+  <si>
+    <t>NTP Servers separated by a comma</t>
   </si>
 </sst>
 </file>
@@ -1180,9 +1192,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{293C1073-CE6E-FC49-B936-0C633F8452D0}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1208,37 +1220,43 @@
         <v>9</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="C2" s="13"/>
+        <v>234</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>97</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="C3" s="13"/>
+        <v>231</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>98</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="C4" s="13"/>
+        <v>231</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1259,7 +1277,9 @@
       <c r="B7" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="13"/>
+      <c r="C7" s="13" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
@@ -1268,7 +1288,9 @@
       <c r="B8" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C8" s="13"/>
+      <c r="C8" s="13" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
@@ -1407,7 +1429,7 @@
         <v>81</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -1418,7 +1440,7 @@
         <v>82</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -1467,226 +1489,226 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D1" t="s">
         <v>175</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>176</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>177</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
+        <v>169</v>
+      </c>
+      <c r="H1" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" s="12" t="s">
         <v>179</v>
-      </c>
-      <c r="F1" t="s">
-        <v>180</v>
-      </c>
-      <c r="G1" t="s">
-        <v>172</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C2" s="13">
         <v>1</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F2" s="14" t="s">
         <v>52</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="H2" s="13"/>
       <c r="I2" s="13"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C3" s="13">
         <v>2</v>
       </c>
       <c r="D3" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="H3" s="14" t="s">
         <v>192</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="I3" s="14" t="s">
         <v>193</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C4" s="13">
         <v>3</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C5" s="13">
         <v>1</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F5" s="14" t="s">
         <v>52</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C6" s="13">
         <v>2</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C7" s="13">
         <v>1</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C8" s="13">
         <v>1</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -1855,9 +1877,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{729B4815-0CB8-AC46-AFED-71170ED8249A}">
   <dimension ref="A1:Z8"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1951,7 +1973,7 @@
       <c r="H2" s="15"/>
       <c r="I2" s="14"/>
       <c r="J2" s="14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K2" s="18" t="s">
         <v>59</v>
@@ -1986,13 +2008,13 @@
       <c r="H3" s="15"/>
       <c r="I3" s="14"/>
       <c r="J3" s="14" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K3" s="18" t="s">
         <v>60</v>
       </c>
       <c r="L3" s="14" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -2021,13 +2043,13 @@
       <c r="H4" s="15"/>
       <c r="I4" s="14"/>
       <c r="J4" s="14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K4" s="18" t="s">
         <v>60</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -2036,16 +2058,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="E5" s="18" t="s">
         <v>109</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>111</v>
       </c>
       <c r="F5" s="15"/>
       <c r="G5" s="15">
@@ -2054,13 +2076,13 @@
       <c r="H5" s="15"/>
       <c r="I5" s="14"/>
       <c r="J5" s="14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K5" s="18" t="s">
         <v>60</v>
       </c>
       <c r="L5" s="14" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -2069,16 +2091,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F6" s="15"/>
       <c r="G6" s="15">
@@ -2087,13 +2109,13 @@
       <c r="H6" s="15"/>
       <c r="I6" s="14"/>
       <c r="J6" s="14" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K6" s="18" t="s">
         <v>60</v>
       </c>
       <c r="L6" s="14" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
@@ -2166,7 +2188,7 @@
         <v>66</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2188,7 +2210,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -2308,31 +2330,31 @@
         <v>8</v>
       </c>
       <c r="B2" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="E2" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="G2" s="14" t="s">
         <v>118</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>120</v>
       </c>
       <c r="H2" s="14" t="s">
         <v>62</v>
       </c>
       <c r="I2" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="K2" s="14" t="s">
         <v>121</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="K2" s="14" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -2341,28 +2363,28 @@
         <v>9</v>
       </c>
       <c r="B3" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="E3" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="F3" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="G3" s="14" t="s">
         <v>127</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>129</v>
       </c>
       <c r="H3" s="14" t="s">
         <v>62</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -2371,28 +2393,28 @@
         <v>10</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>62</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -2474,9 +2496,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B85D48BE-CB72-BC43-A02D-945523B5A1A7}">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="110" zoomScaleNormal="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I14" sqref="I14"/>
+    <sheetView zoomScale="110" zoomScaleNormal="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2498,34 +2520,34 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="F1" t="s">
         <v>134</v>
       </c>
-      <c r="B1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>213</v>
-      </c>
-      <c r="F1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G1" t="s">
-        <v>138</v>
-      </c>
       <c r="H1" s="12" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="I1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="J1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="K1" t="s">
         <v>63</v>
@@ -2534,24 +2556,24 @@
         <v>20</v>
       </c>
       <c r="M1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B2" s="13">
         <v>10000</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D2" s="13">
         <v>100</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F2" s="13">
         <v>10</v>
@@ -2561,16 +2583,16 @@
       </c>
       <c r="H2" s="13"/>
       <c r="I2" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="K2" s="14" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="L2" s="13" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="M2" s="13" t="b">
         <v>1</v>
@@ -2578,13 +2600,13 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B3" s="13">
         <v>10000</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D3" s="13"/>
       <c r="E3" s="13"/>
@@ -2598,16 +2620,16 @@
         <v>50111</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="K3" s="14" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="L3" s="13" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="M3" s="13" t="b">
         <v>1</v>
@@ -2615,13 +2637,13 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B4" s="13">
         <v>10000</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="13"/>
@@ -2633,16 +2655,16 @@
       </c>
       <c r="H4" s="14"/>
       <c r="I4" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="M4" s="13" t="b">
         <v>1</v>
@@ -2650,13 +2672,13 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B5" s="13">
         <v>10000</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -2668,16 +2690,16 @@
       </c>
       <c r="H5" s="14"/>
       <c r="I5" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L5" s="13" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="M5" s="13" t="b">
         <v>1</v>
@@ -2685,13 +2707,13 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B6" s="13">
         <v>10000</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
@@ -2703,16 +2725,16 @@
       </c>
       <c r="H6" s="14"/>
       <c r="I6" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="L6" s="14" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="M6" s="13" t="b">
         <v>1</v>
@@ -2720,13 +2742,13 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B7" s="13">
         <v>10000</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
@@ -2738,16 +2760,16 @@
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="L7" s="14" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="M7" s="13" t="b">
         <v>1</v>
@@ -2755,13 +2777,13 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B8" s="13">
         <v>10000</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
@@ -2773,16 +2795,16 @@
       </c>
       <c r="H8" s="14"/>
       <c r="I8" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="L8" s="14" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="M8" s="13" t="b">
         <v>1</v>
@@ -2790,13 +2812,13 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B9" s="13">
         <v>10000</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
@@ -2808,16 +2830,16 @@
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="L9" s="14" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="M9" s="13" t="b">
         <v>1</v>
@@ -2825,13 +2847,13 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B10" s="13">
         <v>10000</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
@@ -2843,16 +2865,16 @@
       </c>
       <c r="H10" s="14"/>
       <c r="I10" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="K10" s="14" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="L10" s="13" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="M10" s="13" t="b">
         <v>1</v>
@@ -2860,13 +2882,13 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B11" s="13">
         <v>20000</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
@@ -2878,16 +2900,16 @@
       </c>
       <c r="H11" s="13"/>
       <c r="I11" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="K11" s="14" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="L11" s="13" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="M11" s="13" t="b">
         <v>1</v>
@@ -2895,13 +2917,13 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B12" s="13">
         <v>20000</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
@@ -2913,16 +2935,16 @@
       </c>
       <c r="H12" s="13"/>
       <c r="I12" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="K12" s="14" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="L12" s="13" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="M12" s="13" t="b">
         <v>1</v>
@@ -2930,13 +2952,13 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B13" s="13">
         <v>20000</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
@@ -2948,16 +2970,16 @@
       </c>
       <c r="H13" s="13"/>
       <c r="I13" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="K13" s="14" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="L13" s="13" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="M13" s="13" t="b">
         <v>1</v>
@@ -2965,13 +2987,13 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B14" s="13">
         <v>30000</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
@@ -2983,16 +3005,16 @@
       </c>
       <c r="H14" s="13"/>
       <c r="I14" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="K14" s="14" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="L14" s="13" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="M14" s="13" t="b">
         <v>1</v>
@@ -3019,32 +3041,32 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C3" s="14">
         <v>110</v>
@@ -3052,13 +3074,13 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>